<commit_message>
Updated DataPlayground_Dataset_Information Excel Workbook
</commit_message>
<xml_diff>
--- a/DataPlayground_Dataset_Information.xlsx
+++ b/DataPlayground_Dataset_Information.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -97,17 +97,19 @@
     <t xml:space="preserve">https://maven-datasets.s3.amazonaws.com/Movie+Ratings/Rotten+Tomatoes+Movies.csv.zip</t>
   </si>
   <si>
-    <t xml:space="preserve">No</t>
+    <t xml:space="preserve">https://github.com/kjeshang/KunalMavenAnalyticsDataPlayground/blob/main/Movie_Ratings/Logo.png?raw=true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/kjeshang/KunalMavenAnalyticsDataPlayground/tree/main/Movie_Ratings</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy/mm/dd"/>
-    <numFmt numFmtId="166" formatCode="yyyy/mm/dd"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -209,7 +211,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -233,7 +235,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -320,35 +322,41 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>16638</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="H3" s="5" t="n">
+      <c r="H3" s="3" t="n">
         <v>44083</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>24</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="5" t="s">
         <v>25</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -357,6 +365,8 @@
     <hyperlink ref="K2" r:id="rId2" display="https://github.com/kjeshang/KunalMavenAnalyticsDataPlayground/blob/main/INC_5000_Companies/INC_5000_Companies_Logo.jpg?raw=true"/>
     <hyperlink ref="L2" r:id="rId3" display="https://github.com/kjeshang/KunalMavenAnalyticsDataPlayground/tree/main/INC_5000_Companies"/>
     <hyperlink ref="I3" r:id="rId4" display="https://maven-datasets.s3.amazonaws.com/Movie+Ratings/Rotten+Tomatoes+Movies.csv.zip"/>
+    <hyperlink ref="K3" r:id="rId5" display="https://github.com/kjeshang/KunalMavenAnalyticsDataPlayground/blob/main/Movie_Ratings/Logo.png?raw=true"/>
+    <hyperlink ref="L3" r:id="rId6" display="https://github.com/kjeshang/KunalMavenAnalyticsDataPlayground/tree/main/Movie_Ratings"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>